<commit_message>
enter vpn app connection page execution
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/connection/connection_page.xlsx
+++ b/apps/features/backlog/desktop/windows/connection/connection_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\connection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F7DB40-BA45-400F-AC2C-3C562FF9D891}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D37071-2C08-42D2-B90D-125D81451C84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="136">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -607,6 +607,23 @@
   <si>
     <t>download, upload, and ping values should reflect changes after switching to a different server location.</t>
   </si>
+  <si>
+    <t>checking for multiple time clicking</t>
+  </si>
+  <si>
+    <t>TC_SYM_AC_031</t>
+  </si>
+  <si>
+    <t>1. go to microsoftstore and install symlexvpn in the windows.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. navigate to the vpn connection page.
+5. click on "connect" button
+6. checking for multiple time clicking</t>
+  </si>
+  <si>
+    <t>should work perfectly</t>
+  </si>
 </sst>
 </file>
 
@@ -892,14 +909,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -921,6 +930,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1493,7 +1510,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G32" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G33" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1711,8 +1728,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1728,15 +1745,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1758,13 +1775,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2036,7 +2053,7 @@
       <c r="B9" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="18" t="s">
         <v>117</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -2116,7 +2133,7 @@
       <c r="B11" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="19" t="s">
         <v>126</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -2276,7 +2293,7 @@
       <c r="B15" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="19" t="s">
         <v>111</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -2316,7 +2333,7 @@
       <c r="B16" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="19" t="s">
         <v>103</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -2436,7 +2453,7 @@
       <c r="B19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="20" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -2445,8 +2462,8 @@
       <c r="E19" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2474,7 +2491,7 @@
       <c r="B20" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="20" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -2483,8 +2500,8 @@
       <c r="E20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2506,23 +2523,23 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="23" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2544,23 +2561,23 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="23" t="s">
         <v>86</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2582,23 +2599,23 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="24" t="s">
         <v>87</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2620,23 +2637,23 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="24" t="s">
         <v>88</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2658,23 +2675,23 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="24" t="s">
         <v>89</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2696,23 +2713,23 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="24" t="s">
         <v>90</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -2734,23 +2751,23 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="24" t="s">
         <v>84</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -2772,23 +2789,23 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="21" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2810,23 +2827,23 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2848,23 +2865,23 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="130.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="24" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -2886,23 +2903,23 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="21" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -2924,23 +2941,23 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="21" t="s">
         <v>96</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="24" t="s">
         <v>54</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2961,14 +2978,24 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+    <row r="33" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
@@ -29790,7 +29817,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F33" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
crabvpn test and jenkins run
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/connection/connection_page.xlsx
+++ b/apps/features/backlog/desktop/windows/connection/connection_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\connection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6E10E5-7942-4547-BFD5-BF4829EF7D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E62B08C-DA37-4F26-BEEB-FF319DAC90EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -613,9 +613,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>checking for DNS leak</t>
@@ -1851,8 +1848,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2497,10 +2494,10 @@
         <v>71</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>102</v>
@@ -3026,7 +3023,7 @@
         <v>51</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="1"/>
@@ -3066,7 +3063,7 @@
         <v>51</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="1"/>
@@ -3171,19 +3168,19 @@
     </row>
     <row r="34" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="F34" s="13" t="s">
         <v>134</v>
@@ -3211,16 +3208,16 @@
     </row>
     <row r="35" spans="1:26" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>133</v>

</xml_diff>